<commit_message>
Towards processing of performance tables
</commit_message>
<xml_diff>
--- a/inst/extdata/completed-A_performance_table.xlsx
+++ b/inst/extdata/completed-A_performance_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Data\R\dmcda\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DC03E8B-E9AB-4752-BE54-80C93100FD93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3240AE3-4662-4A73-BB55-CC5645BCFEAA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>kitchen</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>Costs</t>
+  </si>
+  <si>
+    <t>digestion</t>
+  </si>
+  <si>
+    <t>Digestion</t>
   </si>
 </sst>
 </file>
@@ -443,13 +449,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="e">
         <v>#N/A</v>
       </c>
@@ -475,10 +487,13 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="e">
         <v>#N/A</v>
       </c>
@@ -504,10 +519,13 @@
         <v>21</v>
       </c>
       <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -520,23 +538,26 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H3" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="e">
-        <v>#N/A</v>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>-1</v>
+      </c>
+      <c r="H3">
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <v>-1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -549,23 +570,26 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="e">
-        <v>#N/A</v>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -578,23 +602,26 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="e">
-        <v>#N/A</v>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>-1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -607,23 +634,26 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H6" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#N/A</v>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -636,23 +666,26 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H7" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I7" t="e">
-        <v>#N/A</v>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -665,20 +698,23 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I8" t="e">
-        <v>#N/A</v>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>